<commit_message>
update workload values added
</commit_message>
<xml_diff>
--- a/Execution_time_energy_Consump_Results.xlsx
+++ b/Execution_time_energy_Consump_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spachava\Downloads\INRAE_M2_Stage_Work_April_August_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554A577A-BC17-420E-86FD-67C81353FB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D9C3BC-8D29-47E0-871C-D8059EC48E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{43B74CA1-C0A7-4870-82BA-6A97DE54515D}"/>
   </bookViews>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8A5405-0C0F-4956-BE0C-4F8184665FE1}">
   <dimension ref="A3:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="I103" sqref="I103"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>